<commit_message>
Adjusted U to T in the usage tables
</commit_message>
<xml_diff>
--- a/human.xlsx
+++ b/human.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\Documents\GitHub\codon_opt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B046C8A5-0839-4CF8-A638-E63C9C4E34C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98E9471-20FE-4B78-8F13-063FDFF777FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{C4B6D569-642A-4EDA-ABF9-2315723504DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,171 +38,72 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
-    <t>UUU</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>UCU</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
-    <t>UUC</t>
-  </si>
-  <si>
-    <t>UCC</t>
-  </si>
-  <si>
-    <t>UUA</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t>UCA</t>
-  </si>
-  <si>
-    <t>UUG</t>
-  </si>
-  <si>
-    <t>UCG</t>
-  </si>
-  <si>
-    <t>CUU</t>
-  </si>
-  <si>
-    <t>CCU</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>CUC</t>
-  </si>
-  <si>
     <t>CCC</t>
   </si>
   <si>
-    <t>CUA</t>
-  </si>
-  <si>
     <t>CCA</t>
   </si>
   <si>
-    <t>CUG</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
-    <t>AUU</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
-    <t>ACU</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
-    <t>AUC</t>
-  </si>
-  <si>
     <t>ACC</t>
   </si>
   <si>
-    <t>AUA</t>
-  </si>
-  <si>
     <t>ACA</t>
   </si>
   <si>
-    <t>AUG</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
     <t>ACG</t>
   </si>
   <si>
-    <t>GUU</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
-    <t>GCU</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>GUC</t>
-  </si>
-  <si>
     <t>GCC</t>
   </si>
   <si>
-    <t>GUA</t>
-  </si>
-  <si>
     <t>GCA</t>
   </si>
   <si>
-    <t>GUG</t>
-  </si>
-  <si>
-    <t>UAU</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>UGU</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>UAC</t>
-  </si>
-  <si>
-    <t>UGC</t>
-  </si>
-  <si>
-    <t>UAA</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
-    <t>UGA</t>
-  </si>
-  <si>
-    <t>UAG</t>
-  </si>
-  <si>
-    <t>UGG</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
-    <t>CAU</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
-    <t>CGU</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -230,15 +131,9 @@
     <t>CGG</t>
   </si>
   <si>
-    <t>AAU</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>AGU</t>
-  </si>
-  <si>
     <t>AAC</t>
   </si>
   <si>
@@ -260,15 +155,9 @@
     <t>AGG</t>
   </si>
   <si>
-    <t>GAU</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
-    <t>GGU</t>
-  </si>
-  <si>
     <t>GAC</t>
   </si>
   <si>
@@ -300,6 +189,117 @@
   </si>
   <si>
     <t>Frequency</t>
+  </si>
+  <si>
+    <t>TTT</t>
+  </si>
+  <si>
+    <t>TTC</t>
+  </si>
+  <si>
+    <t>TTA</t>
+  </si>
+  <si>
+    <t>TTG</t>
+  </si>
+  <si>
+    <t>CTT</t>
+  </si>
+  <si>
+    <t>CTC</t>
+  </si>
+  <si>
+    <t>CTA</t>
+  </si>
+  <si>
+    <t>CTG</t>
+  </si>
+  <si>
+    <t>ATT</t>
+  </si>
+  <si>
+    <t>ATC</t>
+  </si>
+  <si>
+    <t>ATA</t>
+  </si>
+  <si>
+    <t>ATG</t>
+  </si>
+  <si>
+    <t>GTT</t>
+  </si>
+  <si>
+    <t>GTC</t>
+  </si>
+  <si>
+    <t>GTA</t>
+  </si>
+  <si>
+    <t>GTG</t>
+  </si>
+  <si>
+    <t>TCT</t>
+  </si>
+  <si>
+    <t>TCC</t>
+  </si>
+  <si>
+    <t>TCA</t>
+  </si>
+  <si>
+    <t>TCG</t>
+  </si>
+  <si>
+    <t>CCT</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>GCT</t>
+  </si>
+  <si>
+    <t>TAT</t>
+  </si>
+  <si>
+    <t>TAC</t>
+  </si>
+  <si>
+    <t>TAA</t>
+  </si>
+  <si>
+    <t>TAG</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>AAT</t>
+  </si>
+  <si>
+    <t>GAT</t>
+  </si>
+  <si>
+    <t>TGT</t>
+  </si>
+  <si>
+    <t>TGC</t>
+  </si>
+  <si>
+    <t>TGA</t>
+  </si>
+  <si>
+    <t>TGG</t>
+  </si>
+  <si>
+    <t>CGT</t>
+  </si>
+  <si>
+    <t>AGT</t>
+  </si>
+  <si>
+    <t>GGT</t>
   </si>
 </sst>
 </file>
@@ -662,28 +662,28 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
       <c r="C2">
         <v>0.46</v>
@@ -691,10 +691,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0.54</v>
@@ -702,10 +702,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>0.08</v>
@@ -713,10 +713,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>0.13</v>
@@ -724,10 +724,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>0.13</v>
@@ -735,10 +735,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>0.2</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>7.0000000000000007E-2</v>
@@ -757,10 +757,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>0.4</v>
@@ -768,10 +768,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>0.36</v>
@@ -779,10 +779,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>0.47</v>
@@ -790,10 +790,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>0.17</v>
@@ -801,10 +801,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -812,10 +812,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>0.18</v>
@@ -823,10 +823,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>0.24</v>
@@ -834,10 +834,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>0.12</v>
@@ -845,10 +845,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>0.46</v>
@@ -856,10 +856,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0.19</v>
@@ -867,10 +867,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>0.22</v>
@@ -878,10 +878,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0.15</v>
@@ -889,10 +889,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>0.05</v>
@@ -900,10 +900,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>0.28999999999999998</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>0.32</v>
@@ -922,10 +922,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>0.28000000000000003</v>
@@ -933,10 +933,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>0.11</v>
@@ -944,10 +944,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <v>0.25</v>
@@ -955,10 +955,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C27">
         <v>0.36</v>
@@ -966,10 +966,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>0.28000000000000003</v>
@@ -977,10 +977,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C29">
         <v>0.11</v>
@@ -988,10 +988,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>0.27</v>
@@ -999,10 +999,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>0.4</v>
@@ -1010,10 +1010,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>0.23</v>
@@ -1021,10 +1021,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>0.11</v>
@@ -1032,10 +1032,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C34">
         <v>0.44</v>
@@ -1043,10 +1043,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C35">
         <v>0.56000000000000005</v>
@@ -1054,10 +1054,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>0.3</v>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C37">
         <v>0.24</v>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C38">
         <v>0.42</v>
@@ -1087,10 +1087,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C39">
         <v>0.57999999999999996</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C40">
         <v>0.27</v>
@@ -1109,10 +1109,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C41">
         <v>0.73</v>
@@ -1120,10 +1120,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="C42">
         <v>0.47</v>
@@ -1131,10 +1131,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="C43">
         <v>0.53</v>
@@ -1142,10 +1142,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C44">
         <v>0.43</v>
@@ -1153,10 +1153,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C45">
         <v>0.56999999999999995</v>
@@ -1164,10 +1164,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="C46">
         <v>0.46</v>
@@ -1175,10 +1175,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="C47">
         <v>0.54</v>
@@ -1186,10 +1186,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C48">
         <v>0.42</v>
@@ -1197,10 +1197,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C49">
         <v>0.57999999999999996</v>
@@ -1208,10 +1208,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C50">
         <v>0.46</v>
@@ -1219,10 +1219,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C51">
         <v>0.54</v>
@@ -1230,10 +1230,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C52">
         <v>0.47</v>
@@ -1241,10 +1241,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1252,10 +1252,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C54">
         <v>0.08</v>
@@ -1263,10 +1263,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C55">
         <v>0.18</v>
@@ -1274,10 +1274,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C56">
         <v>0.11</v>
@@ -1285,10 +1285,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C57">
         <v>0.2</v>
@@ -1296,10 +1296,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58">
         <v>0.15</v>
@@ -1307,10 +1307,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C59">
         <v>0.24</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C60">
         <v>0.21</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C61">
         <v>0.21</v>
@@ -1340,10 +1340,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C62">
         <v>0.16</v>
@@ -1351,10 +1351,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>0.34</v>
@@ -1362,10 +1362,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <v>0.25</v>
@@ -1373,10 +1373,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>0.25</v>

</xml_diff>